<commit_message>
Adds newly built executable and improvements to batch file
</commit_message>
<xml_diff>
--- a/test/test_file_out.xlsx
+++ b/test/test_file_out.xlsx
@@ -12,6 +12,62 @@
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>1:00pm</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>erics bday</t>
+  </si>
+  <si>
+    <t>2:00pm</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>kelseys bday</t>
+  </si>
+  <si>
+    <t>3:00pm</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>kevins bday</t>
+  </si>
+  <si>
+    <t>4:00pm</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>lelands bday</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -333,7 +389,7 @@
       <selection activeCell="B4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="2.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="9.7109375"/>
@@ -342,123 +398,89 @@
     <col bestFit="1" customWidth="1" max="5" min="5" width="12.28515625"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>31529</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1:00pm</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>erics bday</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>32239</v>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>2:00pm</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>kelseys bday</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>32518</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3:00pm</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>kevins bday</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>32996</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>4:00pm</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>lelands bday</t>
-        </is>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -479,7 +501,7 @@
       <selection activeCell="A1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="2.7109375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="9.7109375"/>
@@ -488,123 +510,89 @@
     <col bestFit="1" customWidth="1" max="5" min="5" width="12.28515625"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>note</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>31529</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1:00pm</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>erics bday</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>32239</v>
       </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>2:00pm</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>kelseys bday</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>32518</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>3:00pm</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>kevins bday</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>32996</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>4:00pm</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>d</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>lelands bday</t>
-        </is>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>